<commit_message>
changed big2.xlsx to 30 flight
</commit_message>
<xml_diff>
--- a/big2.xlsx
+++ b/big2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramb\PycharmProjects\OperationGoed\OperationsMaarDanGoed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DE57261-0240-4681-909A-D0CAD59D19E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13FDB54-F7A2-48B0-99FF-381B9DA4C6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{79B91F4B-CA5E-4A45-AD7D-E616F8CD4CDA}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="107">
   <si>
     <t>Flight no.</t>
   </si>
@@ -159,15 +159,6 @@
     <t>F30</t>
   </si>
   <si>
-    <t>F31</t>
-  </si>
-  <si>
-    <t>F32</t>
-  </si>
-  <si>
-    <t>F33</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -186,81 +177,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>F34</t>
-  </si>
-  <si>
-    <t>F35</t>
-  </si>
-  <si>
-    <t>F36</t>
-  </si>
-  <si>
-    <t>F37</t>
-  </si>
-  <si>
-    <t>F38</t>
-  </si>
-  <si>
-    <t>F39</t>
-  </si>
-  <si>
-    <t>F40</t>
-  </si>
-  <si>
-    <t>F41</t>
-  </si>
-  <si>
-    <t>F42</t>
-  </si>
-  <si>
-    <t>F43</t>
-  </si>
-  <si>
-    <t>F44</t>
-  </si>
-  <si>
-    <t>F45</t>
-  </si>
-  <si>
-    <t>F46</t>
-  </si>
-  <si>
-    <t>F47</t>
-  </si>
-  <si>
-    <t>F48</t>
-  </si>
-  <si>
-    <t>F49</t>
-  </si>
-  <si>
-    <t>F50</t>
-  </si>
-  <si>
-    <t>F51</t>
-  </si>
-  <si>
-    <t>F52</t>
-  </si>
-  <si>
-    <t>F53</t>
-  </si>
-  <si>
-    <t>F54</t>
-  </si>
-  <si>
-    <t>F55</t>
-  </si>
-  <si>
-    <t>F56</t>
-  </si>
-  <si>
-    <t>F57</t>
-  </si>
-  <si>
-    <t>F58</t>
-  </si>
-  <si>
     <t>Gate no.</t>
   </si>
   <si>
@@ -408,66 +324,15 @@
     <t>10:35:00</t>
   </si>
   <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t>11:45:00</t>
-  </si>
-  <si>
     <t>11:55:00</t>
   </si>
   <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
-    <t>12:05:00</t>
-  </si>
-  <si>
-    <t>12:10:00</t>
-  </si>
-  <si>
-    <t>12:15:00</t>
-  </si>
-  <si>
-    <t>12:25:00</t>
-  </si>
-  <si>
-    <t>12:30:00</t>
-  </si>
-  <si>
-    <t>12:35:00</t>
-  </si>
-  <si>
     <t>12:55:00</t>
   </si>
   <si>
-    <t>13:15:00</t>
-  </si>
-  <si>
-    <t>13:25:00</t>
-  </si>
-  <si>
-    <t>13:35:00</t>
-  </si>
-  <si>
     <t>13:40:00</t>
   </si>
   <si>
-    <t>13:50:00</t>
-  </si>
-  <si>
-    <t>13:55:00</t>
-  </si>
-  <si>
-    <t>14:05:00</t>
-  </si>
-  <si>
-    <t>14:15:00</t>
-  </si>
-  <si>
-    <t>14:20:00</t>
-  </si>
-  <si>
     <t>09:35:00</t>
   </si>
   <si>
@@ -490,45 +355,6 @@
   </si>
   <si>
     <t>11:15:00</t>
-  </si>
-  <si>
-    <t>11:50:00</t>
-  </si>
-  <si>
-    <t>13:10:00</t>
-  </si>
-  <si>
-    <t>12:50:00</t>
-  </si>
-  <si>
-    <t>14:50:00</t>
-  </si>
-  <si>
-    <t>14:35:00</t>
-  </si>
-  <si>
-    <t>14:40:00</t>
-  </si>
-  <si>
-    <t>14:55:00</t>
-  </si>
-  <si>
-    <t>15:10:00</t>
-  </si>
-  <si>
-    <t>14:45:00</t>
-  </si>
-  <si>
-    <t>15:25:00</t>
-  </si>
-  <si>
-    <t>15:00:00</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>15:15:00</t>
   </si>
   <si>
     <t>A4</t>
@@ -929,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71DB94B-8C4B-48E9-923F-F1D60482C4C0}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -978,29 +804,29 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="I2">
         <f>SUM(F2:H2)</f>
-        <v>100</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1008,29 +834,29 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="H3">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="I3">
         <f>SUM(F3:H3)</f>
-        <v>150</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1038,29 +864,29 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="H4">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I4">
         <f>SUM(F4:H4)</f>
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1068,29 +894,29 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="H5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I5">
         <f>SUM(F5:H5)</f>
-        <v>50</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1098,29 +924,29 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="H6">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6:I7" si="0">SUM(F6:H6)</f>
-        <v>100</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1128,29 +954,29 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H7">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1158,29 +984,29 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="G8">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="H8">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="I8">
         <f t="shared" ref="I8:I13" si="1">SUM(F8:H8)</f>
-        <v>150</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1188,29 +1014,29 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="F9">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1218,29 +1044,29 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="F10">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="G10">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="H10">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1248,29 +1074,29 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G11">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="H11">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1278,29 +1104,29 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="F12">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="G12">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="H12">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1308,29 +1134,29 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="F13">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="G13">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="H13">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1338,29 +1164,29 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="F14">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="G14">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="H14">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="I14">
         <f t="shared" ref="I14:I15" si="2">SUM(F14:H14)</f>
-        <v>150</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1368,29 +1194,29 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="F15">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="G15">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="H15">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1398,29 +1224,29 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>41</v>
+      </c>
+      <c r="G16">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F16">
-        <v>8</v>
-      </c>
-      <c r="G16">
-        <v>22</v>
-      </c>
       <c r="H16">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="I16">
         <f>SUM(F16:H16)</f>
-        <v>50</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1428,29 +1254,29 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="F17">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="G17">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="H17">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="I17">
         <f t="shared" ref="I17:I18" si="3">SUM(F17:H17)</f>
-        <v>150</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1458,29 +1284,29 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="F18">
-        <v>75</v>
+        <v>139</v>
       </c>
       <c r="G18">
-        <v>25</v>
+        <v>143</v>
       </c>
       <c r="H18">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1488,29 +1314,29 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="F19">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="G19">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="H19">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="I19">
         <f t="shared" ref="I19:I22" si="4">SUM(F19:H19)</f>
-        <v>100</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1518,29 +1344,29 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="F20">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="G20">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="H20">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="I20">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1548,29 +1374,29 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="H21">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="I21">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1578,29 +1404,29 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="F22">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="H22">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="I22">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1608,29 +1434,29 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="F23">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="G23">
-        <v>40</v>
+        <v>143</v>
       </c>
       <c r="H23">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="I23">
         <f t="shared" ref="I23:I28" si="5">SUM(F23:H23)</f>
-        <v>150</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1638,29 +1464,29 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="F24">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G24">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="H24">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="I24">
         <f t="shared" si="5"/>
-        <v>50</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1668,29 +1494,29 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="F25">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G25">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="H25">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="I25">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1698,29 +1524,29 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="F26">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G26">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="H26">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="I26">
         <f t="shared" si="5"/>
-        <v>50</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1728,29 +1554,29 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="F27">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="G27">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="H27">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="I27">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1758,29 +1584,29 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="F28">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="H28">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="I28">
         <f t="shared" si="5"/>
-        <v>150</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1788,29 +1614,29 @@
         <v>36</v>
       </c>
       <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29">
+        <v>28</v>
+      </c>
+      <c r="G29">
+        <v>33</v>
+      </c>
+      <c r="H29">
         <v>44</v>
-      </c>
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F29">
-        <v>7</v>
-      </c>
-      <c r="G29">
-        <v>23</v>
-      </c>
-      <c r="H29">
-        <v>20</v>
       </c>
       <c r="I29">
         <f t="shared" ref="I29:I30" si="6">SUM(F29:H29)</f>
-        <v>50</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1818,29 +1644,29 @@
         <v>37</v>
       </c>
       <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30">
+        <v>33</v>
+      </c>
+      <c r="H30">
         <v>44</v>
-      </c>
-      <c r="C30" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F30">
-        <v>18</v>
-      </c>
-      <c r="G30">
-        <v>17</v>
-      </c>
-      <c r="H30">
-        <v>15</v>
       </c>
       <c r="I30">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1848,870 +1674,142 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="F31">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G31">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="H31">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="I31">
         <f>SUM(F31:H31)</f>
-        <v>100</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="F32">
-        <v>9</v>
-      </c>
-      <c r="G32">
-        <v>26</v>
-      </c>
-      <c r="H32">
-        <v>15</v>
-      </c>
-      <c r="I32">
-        <f>SUM(F32:H32)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33">
-        <v>35</v>
-      </c>
-      <c r="G33">
-        <v>45</v>
-      </c>
-      <c r="H33">
-        <v>20</v>
-      </c>
-      <c r="I33">
-        <f t="shared" ref="I33:I36" si="7">SUM(F33:H33)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34">
-        <v>28</v>
-      </c>
-      <c r="G34">
-        <v>48</v>
-      </c>
-      <c r="H34">
-        <v>24</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" t="s">
-        <v>164</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35">
-        <v>14</v>
-      </c>
-      <c r="G35">
-        <v>37</v>
-      </c>
-      <c r="H35">
-        <v>49</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F36">
-        <v>11</v>
-      </c>
-      <c r="G36">
-        <v>38</v>
-      </c>
-      <c r="H36">
-        <v>51</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F37">
-        <v>7</v>
-      </c>
-      <c r="G37">
-        <v>19</v>
-      </c>
-      <c r="H37">
-        <v>24</v>
-      </c>
-      <c r="I37">
-        <f t="shared" ref="I37:I40" si="8">SUM(F37:H37)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s">
-        <v>164</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F38">
-        <v>11</v>
-      </c>
-      <c r="G38">
-        <v>13</v>
-      </c>
-      <c r="H38">
-        <v>26</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39">
-        <v>13</v>
-      </c>
-      <c r="G39">
-        <v>29</v>
-      </c>
-      <c r="H39">
-        <v>58</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40">
-        <v>47</v>
-      </c>
-      <c r="G40">
-        <v>61</v>
-      </c>
-      <c r="H40">
-        <v>42</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="8"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41">
-        <v>14</v>
-      </c>
-      <c r="G41">
-        <v>17</v>
-      </c>
-      <c r="H41">
-        <v>19</v>
-      </c>
-      <c r="I41">
-        <f t="shared" ref="I41:I53" si="9">SUM(F41:H41)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F42">
-        <v>16</v>
-      </c>
-      <c r="G42">
-        <v>31</v>
-      </c>
-      <c r="H42">
-        <v>53</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>164</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F43">
-        <v>19</v>
-      </c>
-      <c r="G43">
-        <v>28</v>
-      </c>
-      <c r="H43">
-        <v>53</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" t="s">
-        <v>163</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F44">
-        <v>17</v>
-      </c>
-      <c r="G44">
-        <v>32</v>
-      </c>
-      <c r="H44">
-        <v>51</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F45">
-        <v>38</v>
-      </c>
-      <c r="G45">
-        <v>57</v>
-      </c>
-      <c r="H45">
-        <v>55</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46">
-        <v>46</v>
-      </c>
-      <c r="G46">
-        <v>59</v>
-      </c>
-      <c r="H46">
-        <v>45</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" t="s">
-        <v>163</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F47">
-        <v>41</v>
-      </c>
-      <c r="G47">
-        <v>63</v>
-      </c>
-      <c r="H47">
-        <v>46</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F48">
-        <v>37</v>
-      </c>
-      <c r="G48">
-        <v>53</v>
-      </c>
-      <c r="H48">
-        <v>60</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F49">
-        <v>43</v>
-      </c>
-      <c r="G49">
-        <v>64</v>
-      </c>
-      <c r="H49">
-        <v>43</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" t="s">
-        <v>63</v>
-      </c>
-      <c r="B50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" t="s">
-        <v>164</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F50">
-        <v>39</v>
-      </c>
-      <c r="G50">
-        <v>58</v>
-      </c>
-      <c r="H50">
-        <v>53</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51" t="s">
-        <v>163</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F51">
-        <v>44</v>
-      </c>
-      <c r="G51">
-        <v>49</v>
-      </c>
-      <c r="H51">
-        <v>57</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" t="s">
-        <v>65</v>
-      </c>
-      <c r="B52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F52">
-        <v>23</v>
-      </c>
-      <c r="G52">
-        <v>34</v>
-      </c>
-      <c r="H52">
-        <v>43</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" t="s">
-        <v>164</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F53">
-        <v>51</v>
-      </c>
-      <c r="G53">
-        <v>67</v>
-      </c>
-      <c r="H53">
-        <v>32</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="9"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" t="s">
-        <v>42</v>
-      </c>
-      <c r="C54" t="s">
-        <v>164</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F54">
-        <v>21</v>
-      </c>
-      <c r="G54">
-        <v>33</v>
-      </c>
-      <c r="H54">
-        <v>46</v>
-      </c>
-      <c r="I54">
-        <f t="shared" ref="I54:I56" si="10">SUM(F54:H54)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F55">
-        <v>22</v>
-      </c>
-      <c r="G55">
-        <v>39</v>
-      </c>
-      <c r="H55">
-        <v>39</v>
-      </c>
-      <c r="I55">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" t="s">
-        <v>69</v>
-      </c>
-      <c r="B56" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F56">
-        <v>33</v>
-      </c>
-      <c r="G56">
-        <v>61</v>
-      </c>
-      <c r="H56">
-        <v>56</v>
-      </c>
-      <c r="I56">
-        <f t="shared" si="10"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" t="s">
-        <v>70</v>
-      </c>
-      <c r="B57" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F57">
-        <v>18</v>
-      </c>
-      <c r="G57">
-        <v>41</v>
-      </c>
-      <c r="H57">
-        <v>41</v>
-      </c>
-      <c r="I57">
-        <f>SUM(F57:H57)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" t="s">
-        <v>43</v>
-      </c>
-      <c r="C58" t="s">
-        <v>45</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F58">
-        <v>48</v>
-      </c>
-      <c r="G58">
-        <v>56</v>
-      </c>
-      <c r="H58">
-        <v>46</v>
-      </c>
-      <c r="I58">
-        <f>SUM(F58:H58)</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" t="s">
-        <v>42</v>
-      </c>
-      <c r="C59" t="s">
-        <v>46</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F59">
-        <v>26</v>
-      </c>
-      <c r="G59">
-        <v>27</v>
-      </c>
-      <c r="H59">
-        <v>47</v>
-      </c>
-      <c r="I59">
-        <f>SUM(F59:H59)</f>
-        <v>100</v>
-      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="4:5">
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="4:5">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="4:5">
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="4:5">
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="4:5">
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="4:5">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="4:5">
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="4:5">
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="4:5">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="4:5">
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="4:5">
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="4:5">
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="4:5">
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="4:5">
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="4:5">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="4:5">
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="4:5">
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="4:5">
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="4:5">
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="4:5">
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="4:5">
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="4:5">
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="4:5">
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="4:5">
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="4:5">
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I59" xr:uid="{D71DB94B-8C4B-48E9-923F-F1D60482C4C0}"/>
@@ -2725,7 +1823,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2741,33 +1839,33 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>570</v>
@@ -2783,15 +1881,15 @@
         <v>574.66666666666663</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>522</v>
@@ -2807,15 +1905,15 @@
         <v>523.33333333333337</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>555</v>
@@ -2831,15 +1929,15 @@
         <v>549.33333333333337</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>468</v>
@@ -2855,15 +1953,15 @@
         <v>449.66666666666669</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>341</v>
@@ -2879,15 +1977,15 @@
         <v>364</v>
       </c>
       <c r="G6" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>592</v>
@@ -2903,15 +2001,15 @@
         <v>580.66666666666663</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>261</v>
@@ -2927,15 +2025,15 @@
         <v>268</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>379</v>
@@ -2951,15 +2049,15 @@
         <v>363</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>305</v>
@@ -2975,15 +2073,15 @@
         <v>276</v>
       </c>
       <c r="G10" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>274</v>
@@ -2999,15 +2097,15 @@
         <v>295.66666666666669</v>
       </c>
       <c r="G11" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12">
         <v>203</v>
@@ -3023,15 +2121,15 @@
         <v>191.33333333333334</v>
       </c>
       <c r="G12" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>350</v>
@@ -3047,15 +2145,15 @@
         <v>365.33333333333331</v>
       </c>
       <c r="G13" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>271</v>
@@ -3071,15 +2169,15 @@
         <v>285</v>
       </c>
       <c r="G14" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>1208</v>
@@ -3095,15 +2193,15 @@
         <v>1205</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C16">
         <v>1248</v>
@@ -3119,63 +2217,63 @@
         <v>1260.3333333333333</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17">
-        <v>479</v>
+        <v>1473</v>
       </c>
       <c r="D17">
-        <v>468</v>
+        <v>1456</v>
       </c>
       <c r="E17">
-        <v>478</v>
+        <v>1496</v>
       </c>
       <c r="F17" s="3">
         <f>AVERAGE(C17:E17)</f>
-        <v>475</v>
+        <v>1475</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>225</v>
+        <v>1175</v>
       </c>
       <c r="D18">
-        <v>191</v>
+        <v>1224</v>
       </c>
       <c r="E18">
-        <v>237</v>
+        <v>1207</v>
       </c>
       <c r="F18" s="3">
         <f>AVERAGE(C18:E18)</f>
-        <v>217.66666666666666</v>
+        <v>1202</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>958</v>
@@ -3191,55 +2289,55 @@
         <v>971.66666666666663</v>
       </c>
       <c r="G19" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20">
-        <v>1473</v>
+        <v>479</v>
       </c>
       <c r="D20">
-        <v>1456</v>
+        <v>468</v>
       </c>
       <c r="E20">
-        <v>1496</v>
+        <v>478</v>
       </c>
       <c r="F20" s="3">
         <f>AVERAGE(C20:E20)</f>
-        <v>1475</v>
+        <v>475</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21">
-        <v>1175</v>
+        <v>225</v>
       </c>
       <c r="D21">
-        <v>1224</v>
+        <v>191</v>
       </c>
       <c r="E21">
-        <v>1207</v>
+        <v>237</v>
       </c>
       <c r="F21" s="3">
         <f>AVERAGE(C21:E21)</f>
-        <v>1202</v>
+        <v>217.66666666666666</v>
       </c>
       <c r="G21" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>